<commit_message>
Added sheet Merge to Demo1.xlsx Updated Excel Resource file in demo application
</commit_message>
<xml_diff>
--- a/Demo1.xlsx
+++ b/Demo1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Repos\outsystems_advancedexcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5FFE5B-1BC0-4F8F-8C72-488FDC3BC0D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BAB2F4-F746-46EF-8C8B-7EBB250C3A48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo1" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,15 @@
     <sheet name="ShowHide" sheetId="7" r:id="rId7"/>
     <sheet name="ToHide" sheetId="9" r:id="rId8"/>
     <sheet name="ToSetVeryHidden" sheetId="10" r:id="rId9"/>
-    <sheet name="ToUnhide" sheetId="8" state="hidden" r:id="rId10"/>
+    <sheet name="Merge" sheetId="11" r:id="rId10"/>
+    <sheet name="ToUnhide" sheetId="8" state="hidden" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Id</t>
   </si>
@@ -86,6 +87,9 @@
   </si>
   <si>
     <t>Row to show</t>
+  </si>
+  <si>
+    <t>D4 to H8 should be merged…</t>
   </si>
 </sst>
 </file>
@@ -456,37 +460,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="4" spans="1:4" ht="24">
+    <row r="4" spans="1:4" ht="23.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="24">
+    <row r="5" spans="1:4" ht="23.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="24">
+    <row r="6" spans="1:4" ht="23.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="24">
+    <row r="7" spans="1:4" ht="23.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="24">
+    <row r="8" spans="1:4" ht="23.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24">
+    <row r="9" spans="1:4" ht="23.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -499,6 +503,29 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD38A40-D5CE-48E4-AC73-AFEE0942F37B}">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC12A68-2564-4CDC-BCF7-2CD8D9F7F945}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -692,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D442B53-5C9D-482E-B2B9-2D3CE88A45F6}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added UnMerge sheet to Demo1.xlsx
</commit_message>
<xml_diff>
--- a/Demo1.xlsx
+++ b/Demo1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Repos\outsystems_advancedexcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BAB2F4-F746-46EF-8C8B-7EBB250C3A48}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B442785-B823-4C17-9222-B37DD1D28DAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo1" sheetId="1" r:id="rId1"/>
@@ -23,14 +23,15 @@
     <sheet name="ToHide" sheetId="9" r:id="rId8"/>
     <sheet name="ToSetVeryHidden" sheetId="10" r:id="rId9"/>
     <sheet name="Merge" sheetId="11" r:id="rId10"/>
-    <sheet name="ToUnhide" sheetId="8" state="hidden" r:id="rId11"/>
+    <sheet name="UnMerge" sheetId="12" r:id="rId11"/>
+    <sheet name="ToUnhide" sheetId="8" state="hidden" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Id</t>
   </si>
@@ -90,6 +91,9 @@
   </si>
   <si>
     <t>D4 to H8 should be merged…</t>
+  </si>
+  <si>
+    <t>C6 to F11 should be unmerged</t>
   </si>
 </sst>
 </file>
@@ -135,9 +139,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,37 +465,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="4" spans="1:4" ht="23.25">
+    <row r="4" spans="1:4" ht="24">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="23.25">
+    <row r="5" spans="1:4" ht="24">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="23.25">
+    <row r="6" spans="1:4" ht="24">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="23.25">
+    <row r="7" spans="1:4" ht="24">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="23.25">
+    <row r="8" spans="1:4" ht="24">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="23.25">
+    <row r="9" spans="1:4" ht="24">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -506,7 +511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD38A40-D5CE-48E4-AC73-AFEE0942F37B}">
   <dimension ref="B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -526,6 +531,65 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDBC2B16-4A77-46A0-9D26-6B396F421097}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C6:F11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC12A68-2564-4CDC-BCF7-2CD8D9F7F945}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated Demo1.xlsx with UnMerge sheet Updated demo application Generated new .oap versions of extension and demo app for the forge
</commit_message>
<xml_diff>
--- a/Demo1.xlsx
+++ b/Demo1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Repos\outsystems_advancedexcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B442785-B823-4C17-9222-B37DD1D28DAE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6317B7BB-78CB-49F8-97CF-11630032A400}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -532,58 +532,89 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDBC2B16-4A77-46A0-9D26-6B396F421097}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I15" sqref="I15:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:12">
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:12">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:12">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:12">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:12">
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:12">
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
+    <row r="15" spans="1:12">
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="9:12">
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="9:12">
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="9:12">
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C6:F11"/>
+    <mergeCell ref="I15:L19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added the following actions: Row_Delete Column_Insert Column_Delete Comment_Add Comment_Delete
Updated Demo1.xlsx for additional samples

Latest .oap files for upload to the forge
</commit_message>
<xml_diff>
--- a/Demo1.xlsx
+++ b/Demo1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Repos\outsystems_advancedexcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6317B7BB-78CB-49F8-97CF-11630032A400}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EFBE15-7306-4E2A-AE54-8E4E072F5FDD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demo1" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,45 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={0D7E0994-6704-4ED1-B7B6-551AFC03AE10}</author>
+    <author>tc={E08F4EFC-83AA-4C93-8AE9-A685D6B59FDB}</author>
+    <author>tc={4E9BC7D3-CE2C-482F-A595-6FE83621F486}</author>
+  </authors>
+  <commentList>
+    <comment ref="N15" authorId="0" shapeId="0" xr:uid="{0D7E0994-6704-4ED1-B7B6-551AFC03AE10}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This note should be deleted</t>
+      </text>
+    </comment>
+    <comment ref="O17" authorId="1" shapeId="0" xr:uid="{E08F4EFC-83AA-4C93-8AE9-A685D6B59FDB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This should be delted as well.</t>
+      </text>
+    </comment>
+    <comment ref="P18" authorId="2" shapeId="0" xr:uid="{4E9BC7D3-CE2C-482F-A595-6FE83621F486}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This comment should not be deleted.
+Comments in O17 and N15 should have been deleted.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Id</t>
   </si>
@@ -94,13 +131,40 @@
   </si>
   <si>
     <t>C6 to F11 should be unmerged</t>
+  </si>
+  <si>
+    <t>Insert column</t>
+  </si>
+  <si>
+    <t>between I and J</t>
+  </si>
+  <si>
+    <t>Row 7</t>
+  </si>
+  <si>
+    <t>Row 8 - Row 7 is to be deleted</t>
+  </si>
+  <si>
+    <t>Column 1</t>
+  </si>
+  <si>
+    <t>Column 2</t>
+  </si>
+  <si>
+    <t>Column 3</t>
+  </si>
+  <si>
+    <t>should be deleted</t>
+  </si>
+  <si>
+    <t>There should be a comment in K9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -111,6 +175,12 @@
       <sz val="18"/>
       <name val="Book Antiqua"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -158,6 +228,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Hanno Coetzee" id="{9B6B733A-8BF0-4552-A0DE-66FD6BC450B2}" userId="Hanno Coetzee" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -455,55 +531,106 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="N15" dT="2019-06-23T20:13:54.38" personId="{9B6B733A-8BF0-4552-A0DE-66FD6BC450B2}" id="{0D7E0994-6704-4ED1-B7B6-551AFC03AE10}">
+    <text>This note should be deleted</text>
+  </threadedComment>
+  <threadedComment ref="O17" dT="2019-06-23T20:15:57.72" personId="{9B6B733A-8BF0-4552-A0DE-66FD6BC450B2}" id="{E08F4EFC-83AA-4C93-8AE9-A685D6B59FDB}">
+    <text>This should be delted as well.</text>
+  </threadedComment>
+  <threadedComment ref="P18" dT="2019-06-23T20:16:32.35" personId="{9B6B733A-8BF0-4552-A0DE-66FD6BC450B2}" id="{4E9BC7D3-CE2C-482F-A595-6FE83621F486}">
+    <text>This comment should not be deleted.
+Comments in O17 and N15 should have been deleted.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="4" spans="1:4" ht="24">
+    <row r="1" spans="1:17">
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="O2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="24">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="24">
+    <row r="5" spans="1:17" ht="24">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="24">
+    <row r="6" spans="1:17" ht="24">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="24">
-      <c r="A7" s="1"/>
+    <row r="7" spans="1:17" ht="24">
+      <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="24">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:17" ht="24">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="24">
+    <row r="9" spans="1:17" ht="24">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-    </row>
+      <c r="K9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17"/>
+    <row r="17" spans="15:16"/>
+    <row r="18" spans="15:16"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -534,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDBC2B16-4A77-46A0-9D26-6B396F421097}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15:L19"/>
     </sheetView>
   </sheetViews>

</xml_diff>